<commit_message>
adding the data form and annotationson the graph
</commit_message>
<xml_diff>
--- a/data_samples/Realistic Traffic Scenario.xlsx
+++ b/data_samples/Realistic Traffic Scenario.xlsx
@@ -19,33 +19,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
-  <si>
-    <t>Customer ID</t>
-  </si>
-  <si>
-    <t>Event Type</t>
-  </si>
-  <si>
-    <t>Clock Time</t>
-  </si>
-  <si>
-    <t>Service Time</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>Arrival</t>
-  </si>
-  <si>
-    <t>Departure</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>C11</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Service Code</t>
+  </si>
+  <si>
+    <t>Service Title</t>
+  </si>
+  <si>
+    <t>Service Duration (minutes)</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Counseling</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Check-up</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Surgery</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -389,7 +389,7 @@
     <col min="2" max="2" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -399,93 +399,61 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>5</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2">
-        <v>5</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2">
-        <v>4</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2">
-        <v>4</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2">
-        <v>3</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>